<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-1
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pembelajaran dan latihan hitungan dengan mandiri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41AC625-1468-4602-861B-E620A9F3755D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9122454-9208-4EE4-B2F1-573B88DC9197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -467,34 +469,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -537,6 +527,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -852,10 +854,1451 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAD961A-EAA0-475E-9C47-AF31246ECDAA}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>19</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>26</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>24</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>63</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>9</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>83</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>65</v>
+      </c>
+      <c r="J4" s="6">
+        <v>148</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>73</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>49</v>
+      </c>
+      <c r="J5" s="8">
+        <v>122</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>8</v>
+      </c>
+      <c r="J6" s="8">
+        <v>11</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>50</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>9</v>
+      </c>
+      <c r="J7" s="8">
+        <v>59</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>78</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>63</v>
+      </c>
+      <c r="J8" s="8">
+        <v>141</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>71</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>51</v>
+      </c>
+      <c r="J9" s="8">
+        <v>122</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>32</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>55</v>
+      </c>
+      <c r="J10" s="8">
+        <v>87</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>44</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>30</v>
+      </c>
+      <c r="J11" s="8">
+        <v>74</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>93</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>49</v>
+      </c>
+      <c r="J12" s="8">
+        <v>142</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>8</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>85</v>
+      </c>
+      <c r="J13" s="8">
+        <v>93</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>91</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>60</v>
+      </c>
+      <c r="J14" s="10">
+        <v>151</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>72</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>33</v>
+      </c>
+      <c r="J20" s="14">
+        <v>39</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>66</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>67</v>
+      </c>
+      <c r="J21" s="18">
+        <v>-1</v>
+      </c>
+      <c r="K21" s="11">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>23</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>38</v>
+      </c>
+      <c r="J22" s="18">
+        <v>-15</v>
+      </c>
+      <c r="K22" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>8</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>3</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>45</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>51</v>
+      </c>
+      <c r="J23" s="18">
+        <v>-6</v>
+      </c>
+      <c r="K23" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>5</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>27</v>
+      </c>
+      <c r="J24" s="18">
+        <v>-22</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>95</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>85</v>
+      </c>
+      <c r="J25" s="18">
+        <v>10</v>
+      </c>
+      <c r="K25" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>14</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>84</v>
+      </c>
+      <c r="J26" s="18">
+        <v>-70</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>88</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>50</v>
+      </c>
+      <c r="J27" s="18">
+        <v>38</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>75</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>41</v>
+      </c>
+      <c r="J28" s="18">
+        <v>34</v>
+      </c>
+      <c r="K28" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>7</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>81</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-74</v>
+      </c>
+      <c r="K29" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>95</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>1</v>
+      </c>
+      <c r="J30" s="22">
+        <v>94</v>
+      </c>
+      <c r="K30" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>27</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>9</v>
+      </c>
+      <c r="J36" s="14">
+        <v>243</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>2</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>15</v>
+      </c>
+      <c r="J37" s="18">
+        <v>30</v>
+      </c>
+      <c r="K37" s="11">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>20</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>28</v>
+      </c>
+      <c r="J38" s="18">
+        <v>560</v>
+      </c>
+      <c r="K38" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>20</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>5</v>
+      </c>
+      <c r="J39" s="18">
+        <v>100</v>
+      </c>
+      <c r="K39" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>28</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>2</v>
+      </c>
+      <c r="J40" s="18">
+        <v>56</v>
+      </c>
+      <c r="K40" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>15</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>1</v>
+      </c>
+      <c r="J41" s="18">
+        <v>15</v>
+      </c>
+      <c r="K41" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>11</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>30</v>
+      </c>
+      <c r="J42" s="18">
+        <v>330</v>
+      </c>
+      <c r="K42" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>20</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>22</v>
+      </c>
+      <c r="J43" s="18">
+        <v>440</v>
+      </c>
+      <c r="K43" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>23</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>12</v>
+      </c>
+      <c r="J44" s="18">
+        <v>276</v>
+      </c>
+      <c r="K44" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>2</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>22</v>
+      </c>
+      <c r="J45" s="18">
+        <v>44</v>
+      </c>
+      <c r="K45" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>4</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>24</v>
+      </c>
+      <c r="J46" s="22">
+        <v>96</v>
+      </c>
+      <c r="K46" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>25</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>9</v>
+      </c>
+      <c r="J52" s="23">
+        <v>2.78</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>29</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>20</v>
+      </c>
+      <c r="J53" s="18">
+        <v>1.45</v>
+      </c>
+      <c r="K53" s="11">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>19</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>15</v>
+      </c>
+      <c r="J54" s="18">
+        <v>1.27</v>
+      </c>
+      <c r="K54" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>8</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>3</v>
+      </c>
+      <c r="J55" s="18">
+        <v>2.67</v>
+      </c>
+      <c r="K55" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>1</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>10</v>
+      </c>
+      <c r="J56" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="K56" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>8</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>28</v>
+      </c>
+      <c r="J57" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="K57" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>15</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>27</v>
+      </c>
+      <c r="J58" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K58" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>19</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>19</v>
+      </c>
+      <c r="J59" s="18">
+        <v>1</v>
+      </c>
+      <c r="K59" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>8</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>30</v>
+      </c>
+      <c r="J60" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="K60" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>30</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>26</v>
+      </c>
+      <c r="J61" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K61" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>28</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>7</v>
+      </c>
+      <c r="J62" s="22">
+        <v>4</v>
+      </c>
+      <c r="K62" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{BB61DC7E-0494-4EFE-83E2-9CEC11594A9E}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{F737F39E-A80B-448F-94E3-ECF8771402EB}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{285E40A3-562E-46D1-A099-27D7510AD07F}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{B7A746AF-18FF-4597-B0B7-6D9DBC6F7148}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -870,26 +2313,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -898,32 +2341,32 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>15</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="31" t="s">
         <v>7</v>
       </c>
     </row>
@@ -934,15 +2377,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -972,15 +2415,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1005,11 +2448,11 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -1038,15 +2481,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1071,15 +2514,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1104,15 +2547,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1137,15 +2580,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1170,15 +2613,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1203,15 +2646,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1236,15 +2679,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1280,53 +2723,53 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="26" t="s">
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="K19" s="24" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="37">
         <f>COUNTIF($K$4:$K$14,1)</f>
         <v>1</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="43">
         <f>COUNTIF($K$4:$K$14,0)</f>
         <v>0</v>
       </c>
@@ -1352,14 +2795,14 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="38">
         <f>COUNTIF($K$20:$K$30,1)</f>
         <v>1</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="44">
         <f>COUNTIF($K$20:$K$30,0)</f>
         <v>0</v>
       </c>
@@ -1380,14 +2823,14 @@
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="38">
         <f>COUNTIF($K$36:$K$46,1)</f>
         <v>1</v>
       </c>
-      <c r="D22" s="48">
+      <c r="D22" s="44">
         <f>COUNTIF($K$36:$K$46,0)</f>
         <v>0</v>
       </c>
@@ -1408,14 +2851,14 @@
       <c r="K22" s="15"/>
     </row>
     <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="39">
         <f>COUNTIF($K$52:$K$62,1)</f>
         <v>1</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="45">
         <f>COUNTIF($K$52:$K$62,0)</f>
         <v>0</v>
       </c>
@@ -1555,32 +2998,32 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="30" t="s">
+      <c r="F34" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="F35" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="G35" s="32" t="s">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="31" t="s">
+      <c r="H35" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I35" s="32" t="s">
+      <c r="I35" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J35" s="32" t="s">
+      <c r="J35" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="K35" s="31" t="s">
+      <c r="K35" s="28" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1777,32 +3220,32 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="27" t="s">
+      <c r="F50" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="F51" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="G51" s="29" t="s">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H51" s="28" t="s">
+      <c r="H51" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I51" s="29" t="s">
+      <c r="I51" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J51" s="29" t="s">
+      <c r="J51" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K51" s="28" t="s">
+      <c r="K51" s="26" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-2
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9122454-9208-4EE4-B2F1-573B88DC9197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9866C-9E6B-49DB-A24D-6736E2634904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Hari Ke-2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Hari Ke-2'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -404,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,6 +529,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -857,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAD961A-EAA0-475E-9C47-AF31246ECDAA}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -884,14 +898,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -900,15 +914,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -936,15 +950,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -974,15 +988,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1012,15 +1026,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1050,15 +1064,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1088,15 +1102,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1126,15 +1140,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1164,15 +1178,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1202,11 +1216,11 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -1240,15 +1254,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1278,15 +1292,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1332,14 +1346,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1657,14 +1671,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="48" t="s">
+      <c r="F34" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -1929,14 +1943,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="49" t="s">
+      <c r="F50" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2295,10 +2309,1451 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4C9E2B-E030-44CC-B4EC-B79CD7EBCABE}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>45</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>11</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>46</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2">
+        <v>13</v>
+      </c>
+      <c r="J4" s="6">
+        <v>59</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>58</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3">
+        <v>12</v>
+      </c>
+      <c r="J5" s="8">
+        <v>70</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>60</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="3">
+        <v>57</v>
+      </c>
+      <c r="J6" s="8">
+        <v>117</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>49</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="3">
+        <v>26</v>
+      </c>
+      <c r="J7" s="8">
+        <v>75</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>97</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="3">
+        <v>46</v>
+      </c>
+      <c r="J8" s="8">
+        <v>143</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3">
+        <v>89</v>
+      </c>
+      <c r="J9" s="8">
+        <v>94</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="3">
+        <v>17</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>95</v>
+      </c>
+      <c r="J10" s="8">
+        <v>112</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>69</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="3">
+        <v>57</v>
+      </c>
+      <c r="J11" s="8">
+        <v>126</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="3">
+        <v>45</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>47</v>
+      </c>
+      <c r="J12" s="8">
+        <v>92</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="3">
+        <v>67</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8">
+        <v>69</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="4">
+        <v>83</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="4">
+        <v>26</v>
+      </c>
+      <c r="J14" s="10">
+        <v>109</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>17</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>85</v>
+      </c>
+      <c r="J20" s="14">
+        <v>-68</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>78</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>24</v>
+      </c>
+      <c r="J21" s="18">
+        <v>54</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>43</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>90</v>
+      </c>
+      <c r="J22" s="18">
+        <v>-47</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>7</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>4</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>95</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>19</v>
+      </c>
+      <c r="J23" s="18">
+        <v>76</v>
+      </c>
+      <c r="K23" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>73</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>22</v>
+      </c>
+      <c r="J24" s="18">
+        <v>51</v>
+      </c>
+      <c r="K24" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>92</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>80</v>
+      </c>
+      <c r="J25" s="18">
+        <v>12</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>52</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>98</v>
+      </c>
+      <c r="J26" s="18">
+        <v>-46</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>49</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>33</v>
+      </c>
+      <c r="J27" s="18">
+        <v>16</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>7</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>69</v>
+      </c>
+      <c r="J28" s="18">
+        <v>-62</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>22</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>88</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-66</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>75</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>35</v>
+      </c>
+      <c r="J30" s="22">
+        <v>40</v>
+      </c>
+      <c r="K30" s="19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>6</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>2</v>
+      </c>
+      <c r="J36" s="14">
+        <v>12</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>21</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>22</v>
+      </c>
+      <c r="J37" s="18">
+        <v>462</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>8</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>19</v>
+      </c>
+      <c r="J38" s="18">
+        <v>152</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>24</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>1</v>
+      </c>
+      <c r="J39" s="18">
+        <v>24</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>28</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>21</v>
+      </c>
+      <c r="J40" s="18">
+        <v>588</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>29</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>22</v>
+      </c>
+      <c r="J41" s="18">
+        <v>638</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>2</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>10</v>
+      </c>
+      <c r="J42" s="18">
+        <v>20</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>28</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>27</v>
+      </c>
+      <c r="J43" s="18">
+        <v>756</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>5</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>17</v>
+      </c>
+      <c r="J44" s="18">
+        <v>85</v>
+      </c>
+      <c r="K44" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>10</v>
+      </c>
+      <c r="J45" s="18">
+        <v>10</v>
+      </c>
+      <c r="K45" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>6</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>4</v>
+      </c>
+      <c r="J46" s="22">
+        <v>24</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>11</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>25</v>
+      </c>
+      <c r="J52" s="23">
+        <v>0.44</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>10</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>24</v>
+      </c>
+      <c r="J53" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>15</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>25</v>
+      </c>
+      <c r="J54" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="K54" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>25</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>3</v>
+      </c>
+      <c r="J55" s="18">
+        <v>8.33</v>
+      </c>
+      <c r="K55" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>18</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>6</v>
+      </c>
+      <c r="J56" s="18">
+        <v>3</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>26</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>1</v>
+      </c>
+      <c r="J57" s="18">
+        <v>26</v>
+      </c>
+      <c r="K57" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>20</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>29</v>
+      </c>
+      <c r="J58" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="K58" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>10</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>14</v>
+      </c>
+      <c r="J59" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>27</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>30</v>
+      </c>
+      <c r="J60" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="K60" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>15</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>19</v>
+      </c>
+      <c r="J61" s="18">
+        <v>0.79</v>
+      </c>
+      <c r="K61" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>10</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>25</v>
+      </c>
+      <c r="J62" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{789DEF8F-7F5B-4746-9306-DA5E7BF33E1B}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{DA1A219E-EF7F-4CC4-B192-1599E93AC50E}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{323352D9-EE5D-47F9-AD9D-DF8C2AB6373C}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{DFBCDF90-CAB5-4448-ABB5-8F810BDB9DDB}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView topLeftCell="B48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -2325,14 +3780,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2341,15 +3796,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -2377,15 +3832,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2415,15 +3870,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2448,15 +3903,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2481,15 +3936,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2514,15 +3969,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2547,15 +4002,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2580,15 +4035,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>3</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>7</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2613,15 +4068,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2646,15 +4101,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2679,15 +4134,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2723,14 +4178,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -2998,14 +4453,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="48" t="s">
+      <c r="F34" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3220,14 +4675,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="49" t="s">
+      <c r="F50" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-3
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9866C-9E6B-49DB-A24D-6736E2634904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225E99B5-A308-4AF2-A876-6DA2DD63AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
     <sheet name="Hari Ke-2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hari Ke-3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Hari Ke-2'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Hari Ke-3'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -406,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,6 +555,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -898,14 +915,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -914,15 +931,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -950,15 +967,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -988,15 +1005,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1026,15 +1043,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1064,15 +1081,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1102,15 +1119,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1140,15 +1157,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1178,15 +1195,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1216,15 +1233,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>11</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>26</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1254,15 +1271,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1292,15 +1309,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1346,14 +1363,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="51" t="s">
+      <c r="F18" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1671,14 +1688,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="52" t="s">
+      <c r="F34" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -1943,14 +1960,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="53" t="s">
+      <c r="F50" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2312,7 +2329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4C9E2B-E030-44CC-B4EC-B79CD7EBCABE}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -2339,14 +2356,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2355,7 +2372,7 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
@@ -2363,7 +2380,7 @@
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>1</v>
@@ -2391,15 +2408,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2429,15 +2446,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2467,15 +2484,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2505,15 +2522,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2543,15 +2560,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2581,15 +2598,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2619,15 +2636,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2657,15 +2674,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2695,15 +2712,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2733,15 +2750,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2787,14 +2804,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="51" t="s">
+      <c r="F18" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -3112,14 +3129,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="52" t="s">
+      <c r="F34" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3384,14 +3401,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="53" t="s">
+      <c r="F50" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -3750,6 +3767,1447 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BC5746-7883-4546-8887-15FB02EF52B0}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>37</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>18</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>17</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>49</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>64</v>
+      </c>
+      <c r="J4" s="6">
+        <v>113</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>46</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>71</v>
+      </c>
+      <c r="J5" s="8">
+        <v>117</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>17</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>93</v>
+      </c>
+      <c r="J6" s="8">
+        <v>110</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>38</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>26</v>
+      </c>
+      <c r="J7" s="8">
+        <v>64</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>83</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>71</v>
+      </c>
+      <c r="J8" s="8">
+        <v>154</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>93</v>
+      </c>
+      <c r="J9" s="8">
+        <v>136</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>19</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>84</v>
+      </c>
+      <c r="J10" s="8">
+        <v>103</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>77</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>97</v>
+      </c>
+      <c r="J11" s="8">
+        <v>174</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>10</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>77</v>
+      </c>
+      <c r="J12" s="8">
+        <v>87</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>47</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>72</v>
+      </c>
+      <c r="J13" s="8">
+        <v>119</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>96</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>15</v>
+      </c>
+      <c r="J14" s="10">
+        <v>111</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>72</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>22</v>
+      </c>
+      <c r="J20" s="14">
+        <v>50</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>82</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>61</v>
+      </c>
+      <c r="J21" s="18">
+        <v>21</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>63</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>28</v>
+      </c>
+      <c r="J22" s="18">
+        <v>35</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>9</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>36</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>12</v>
+      </c>
+      <c r="J23" s="18">
+        <v>24</v>
+      </c>
+      <c r="K23" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>64</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>95</v>
+      </c>
+      <c r="J24" s="18">
+        <v>-31</v>
+      </c>
+      <c r="K24" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>23</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>18</v>
+      </c>
+      <c r="J25" s="18">
+        <v>5</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>52</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>64</v>
+      </c>
+      <c r="J26" s="18">
+        <v>-12</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>69</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>47</v>
+      </c>
+      <c r="J27" s="18">
+        <v>22</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>34</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>35</v>
+      </c>
+      <c r="J28" s="18">
+        <v>-1</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>6</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>30</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-24</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>8</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>34</v>
+      </c>
+      <c r="J30" s="22">
+        <v>-26</v>
+      </c>
+      <c r="K30" s="19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>17</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>23</v>
+      </c>
+      <c r="J36" s="14">
+        <v>391</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>1</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>23</v>
+      </c>
+      <c r="J37" s="18">
+        <v>23</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>14</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>28</v>
+      </c>
+      <c r="J38" s="18">
+        <v>392</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>16</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>7</v>
+      </c>
+      <c r="J39" s="18">
+        <v>112</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>6</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>9</v>
+      </c>
+      <c r="J40" s="18">
+        <v>54</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>24</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>13</v>
+      </c>
+      <c r="J41" s="18">
+        <v>312</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>25</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>9</v>
+      </c>
+      <c r="J42" s="18">
+        <v>225</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>13</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>5</v>
+      </c>
+      <c r="J43" s="18">
+        <v>65</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>26</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>20</v>
+      </c>
+      <c r="J44" s="18">
+        <v>520</v>
+      </c>
+      <c r="K44" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>5</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>7</v>
+      </c>
+      <c r="J45" s="18">
+        <v>35</v>
+      </c>
+      <c r="K45" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>14</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>12</v>
+      </c>
+      <c r="J46" s="22">
+        <v>168</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>23</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>23</v>
+      </c>
+      <c r="J52" s="23">
+        <v>1</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>17</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>21</v>
+      </c>
+      <c r="J53" s="18">
+        <v>0.89</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>12</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>28</v>
+      </c>
+      <c r="J54" s="18">
+        <v>0.43</v>
+      </c>
+      <c r="K54" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>25</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>16</v>
+      </c>
+      <c r="J55" s="18">
+        <v>1.56</v>
+      </c>
+      <c r="K55" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>11</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>13</v>
+      </c>
+      <c r="J56" s="18">
+        <v>0.85</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>27</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>14</v>
+      </c>
+      <c r="J57" s="18">
+        <v>1.93</v>
+      </c>
+      <c r="K57" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>4</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>13</v>
+      </c>
+      <c r="J58" s="58">
+        <v>0.38</v>
+      </c>
+      <c r="K58" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>10</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>9</v>
+      </c>
+      <c r="J59" s="18">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>25</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>11</v>
+      </c>
+      <c r="J60" s="18">
+        <v>2.27</v>
+      </c>
+      <c r="K60" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>27</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>30</v>
+      </c>
+      <c r="J61" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="K61" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>26</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>2</v>
+      </c>
+      <c r="J62" s="22">
+        <v>13</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{BD3F794D-BA78-4800-A711-D7033CDB4C7B}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{01AE88E9-F15C-4600-BA7E-31355ED2A58D}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{24EAAE22-64DF-494E-BC4D-21C5EADF2D67}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{08CED535-9070-4CA5-8E55-68DB623F665A}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
@@ -3780,14 +5238,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3796,15 +5254,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -3832,15 +5290,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -3870,15 +5328,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -3903,15 +5361,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -3940,11 +5398,11 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -3969,15 +5427,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -4002,15 +5460,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -4039,11 +5497,11 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -4068,15 +5526,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -4101,15 +5559,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -4134,15 +5592,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -4178,14 +5636,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="51" t="s">
+      <c r="F18" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -4453,14 +5911,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="52" t="s">
+      <c r="F34" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="56"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -4675,14 +6133,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="53" t="s">
+      <c r="F50" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-4
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225E99B5-A308-4AF2-A876-6DA2DD63AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61BF6EC-1CC8-4BE3-BA36-5F4783D87144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
     <sheet name="Hari Ke-2" sheetId="3" r:id="rId2"/>
     <sheet name="Hari Ke-3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hari Ke-4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Hari Ke-2'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Hari Ke-3'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Hari Ke-4'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -408,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -570,6 +572,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -888,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAD961A-EAA0-475E-9C47-AF31246ECDAA}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="B43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,14 +929,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -931,15 +945,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -967,15 +981,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -1005,15 +1019,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1043,15 +1057,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1081,7 +1095,7 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -1089,7 +1103,7 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1119,15 +1133,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1157,15 +1171,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1195,15 +1209,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1233,7 +1247,7 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -1241,7 +1255,7 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1271,15 +1285,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1309,15 +1323,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1363,14 +1377,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1688,14 +1702,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -1960,14 +1974,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="57" t="s">
+      <c r="F50" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2356,14 +2370,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2372,15 +2386,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>1</v>
@@ -2408,15 +2422,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2446,15 +2460,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2484,15 +2498,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2522,15 +2536,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2560,15 +2574,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2598,15 +2612,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2636,15 +2650,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2674,15 +2688,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2712,15 +2726,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2750,15 +2764,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2804,14 +2818,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -3129,14 +3143,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3401,14 +3415,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="57" t="s">
+      <c r="F50" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -3770,7 +3784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BC5746-7883-4546-8887-15FB02EF52B0}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -3797,14 +3811,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3813,15 +3827,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>1</v>
@@ -3849,15 +3863,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -3887,15 +3901,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -3925,15 +3939,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -3963,15 +3977,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -4001,15 +4015,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -4039,15 +4053,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -4077,15 +4091,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -4115,15 +4129,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -4153,15 +4167,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -4191,15 +4205,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -4245,14 +4259,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -4570,14 +4584,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -4842,14 +4856,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="57" t="s">
+      <c r="F50" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -5208,6 +5222,1447 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3F6CA9-EAB4-411B-BB42-7EA341FC2E42}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>32</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>12</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>78</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>34</v>
+      </c>
+      <c r="J4" s="6">
+        <v>37</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>95</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>21</v>
+      </c>
+      <c r="J5" s="8">
+        <v>116</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>20</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>74</v>
+      </c>
+      <c r="J6" s="8">
+        <v>94</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>69</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>37</v>
+      </c>
+      <c r="J7" s="8">
+        <v>106</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>45</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>32</v>
+      </c>
+      <c r="J8" s="8">
+        <v>77</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>19</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>31</v>
+      </c>
+      <c r="J9" s="8">
+        <v>50</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>45</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>53</v>
+      </c>
+      <c r="J10" s="8">
+        <v>98</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>49</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>97</v>
+      </c>
+      <c r="J11" s="8">
+        <v>146</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>4</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>84</v>
+      </c>
+      <c r="J12" s="8">
+        <v>88</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>59</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>25</v>
+      </c>
+      <c r="J13" s="8">
+        <v>84</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>14</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>23</v>
+      </c>
+      <c r="J14" s="10">
+        <v>37</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>18</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>65</v>
+      </c>
+      <c r="J20" s="14">
+        <v>-47</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>18</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>79</v>
+      </c>
+      <c r="J21" s="18">
+        <v>-61</v>
+      </c>
+      <c r="K21" s="11">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>88</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>70</v>
+      </c>
+      <c r="J22" s="18">
+        <v>18</v>
+      </c>
+      <c r="K22" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>10</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>74</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>59</v>
+      </c>
+      <c r="J23" s="18">
+        <v>15</v>
+      </c>
+      <c r="K23" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>47</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>72</v>
+      </c>
+      <c r="J24" s="18">
+        <v>-25</v>
+      </c>
+      <c r="K24" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>16</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>90</v>
+      </c>
+      <c r="J25" s="18">
+        <v>-74</v>
+      </c>
+      <c r="K25" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>12</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>53</v>
+      </c>
+      <c r="J26" s="18">
+        <v>-41</v>
+      </c>
+      <c r="K26" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>29</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>61</v>
+      </c>
+      <c r="J27" s="18">
+        <v>-32</v>
+      </c>
+      <c r="K27" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>53</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>96</v>
+      </c>
+      <c r="J28" s="18">
+        <v>-43</v>
+      </c>
+      <c r="K28" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>40</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>40</v>
+      </c>
+      <c r="J29" s="18">
+        <v>0</v>
+      </c>
+      <c r="K29" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>20</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>82</v>
+      </c>
+      <c r="J30" s="22">
+        <v>-62</v>
+      </c>
+      <c r="K30" s="11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>6</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>22</v>
+      </c>
+      <c r="J36" s="14">
+        <v>132</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>1</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>28</v>
+      </c>
+      <c r="J37" s="18">
+        <v>28</v>
+      </c>
+      <c r="K37" s="11">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>18</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>27</v>
+      </c>
+      <c r="J38" s="18">
+        <v>486</v>
+      </c>
+      <c r="K38" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>4</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>30</v>
+      </c>
+      <c r="J39" s="18">
+        <v>120</v>
+      </c>
+      <c r="K39" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>3</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>9</v>
+      </c>
+      <c r="J40" s="18">
+        <v>27</v>
+      </c>
+      <c r="K40" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>22</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>5</v>
+      </c>
+      <c r="J41" s="18">
+        <v>110</v>
+      </c>
+      <c r="K41" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>18</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>21</v>
+      </c>
+      <c r="J42" s="18">
+        <v>378</v>
+      </c>
+      <c r="K42" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>26</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>30</v>
+      </c>
+      <c r="J43" s="18">
+        <v>780</v>
+      </c>
+      <c r="K43" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>29</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>10</v>
+      </c>
+      <c r="J44" s="18">
+        <v>290</v>
+      </c>
+      <c r="K44" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>8</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>7</v>
+      </c>
+      <c r="J45" s="18">
+        <v>56</v>
+      </c>
+      <c r="K45" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>29</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>23</v>
+      </c>
+      <c r="J46" s="22">
+        <v>667</v>
+      </c>
+      <c r="K46" s="11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>29</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>15</v>
+      </c>
+      <c r="J52" s="23">
+        <v>1.93</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>15</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>4</v>
+      </c>
+      <c r="J53" s="18">
+        <v>3.75</v>
+      </c>
+      <c r="K53" s="11">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>25</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>12</v>
+      </c>
+      <c r="J54" s="18">
+        <v>2.84</v>
+      </c>
+      <c r="K54" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>12</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>20</v>
+      </c>
+      <c r="J55" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="K55" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>9</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>23</v>
+      </c>
+      <c r="J56" s="18">
+        <v>0.39</v>
+      </c>
+      <c r="K56" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>11</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>29</v>
+      </c>
+      <c r="J57" s="18">
+        <v>0.38</v>
+      </c>
+      <c r="K57" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>7</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>4</v>
+      </c>
+      <c r="J58" s="18">
+        <v>1.75</v>
+      </c>
+      <c r="K58" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>4</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>9</v>
+      </c>
+      <c r="J59" s="18">
+        <v>0.44</v>
+      </c>
+      <c r="K59" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>24</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>4</v>
+      </c>
+      <c r="J60" s="18">
+        <v>6</v>
+      </c>
+      <c r="K60" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>15</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>11</v>
+      </c>
+      <c r="J61" s="18">
+        <v>1.36</v>
+      </c>
+      <c r="K61" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>18</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>11</v>
+      </c>
+      <c r="J62" s="22">
+        <v>1.64</v>
+      </c>
+      <c r="K62" s="11">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{72FBC709-C31F-454A-9B22-8466A3A9F592}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{E27E7AD1-7AAD-4206-8FBF-6544595CD8F6}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{2520F550-4B80-4CD6-B6D5-1191D4526433}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{F9F25FEF-A1DE-413C-8179-CCFD24280A76}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
@@ -5238,14 +6693,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5254,15 +6709,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -5290,15 +6745,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -5328,15 +6783,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -5361,15 +6816,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -5394,15 +6849,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -5427,15 +6882,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -5460,15 +6915,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -5493,15 +6948,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -5526,15 +6981,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -5559,7 +7014,7 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -5567,7 +7022,7 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -5592,15 +7047,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -5636,14 +7091,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -5911,14 +7366,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -6133,14 +7588,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="57" t="s">
+      <c r="F50" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-5
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61BF6EC-1CC8-4BE3-BA36-5F4783D87144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCD07C1-739A-485B-9256-3F7995FC9D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
     <sheet name="Hari Ke-2" sheetId="3" r:id="rId2"/>
     <sheet name="Hari Ke-3" sheetId="4" r:id="rId3"/>
     <sheet name="Hari Ke-4" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Hari Ke-5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Hari Ke-2'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Hari Ke-3'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Hari Ke-4'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Hari Ke-5'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -410,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -572,6 +574,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -929,14 +943,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -945,11 +959,11 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
@@ -981,15 +995,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -1019,15 +1033,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1057,15 +1071,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1095,15 +1109,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1133,15 +1147,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1171,15 +1185,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1209,15 +1223,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1247,15 +1261,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1285,15 +1299,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1323,15 +1337,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1377,14 +1391,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1702,14 +1716,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="61" t="s">
+      <c r="F34" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -1974,14 +1988,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2370,14 +2384,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2386,15 +2400,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>1</v>
@@ -2422,15 +2436,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2460,15 +2474,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2498,15 +2512,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2536,15 +2550,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2574,15 +2588,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2612,15 +2626,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2650,15 +2664,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2688,15 +2702,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2726,15 +2740,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2764,15 +2778,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2818,14 +2832,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -3143,14 +3157,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="61" t="s">
+      <c r="F34" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3415,14 +3429,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -3811,14 +3825,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3827,15 +3841,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>1</v>
@@ -3863,15 +3877,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -3901,15 +3915,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -3939,15 +3953,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -3977,15 +3991,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -4015,15 +4029,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>22</v>
       </c>
-      <c r="C8" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>24</v>
-      </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -4053,15 +4067,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -4091,15 +4105,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -4129,15 +4143,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -4167,15 +4181,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -4205,15 +4219,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -4259,14 +4273,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -4584,14 +4598,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="61" t="s">
+      <c r="F34" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -4856,14 +4870,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -5225,7 +5239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3F6CA9-EAB4-411B-BB42-7EA341FC2E42}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
@@ -5252,14 +5266,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5268,15 +5282,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F3" s="54" t="s">
         <v>1</v>
@@ -5304,15 +5318,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -5342,15 +5356,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -5380,15 +5394,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -5418,15 +5432,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -5456,15 +5470,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -5494,15 +5508,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -5532,15 +5546,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -5570,7 +5584,7 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -5578,7 +5592,7 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -5608,15 +5622,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -5646,15 +5660,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -5700,14 +5714,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -6025,14 +6039,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="61" t="s">
+      <c r="F34" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -6297,14 +6311,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -6663,6 +6677,1447 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA416E0B-43CD-4AE8-B502-D513E78B933D}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>60</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>23</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>15</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>55</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6">
+        <v>58</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>97</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>90</v>
+      </c>
+      <c r="J5" s="8">
+        <v>187</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>70</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>80</v>
+      </c>
+      <c r="J6" s="8">
+        <v>150</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>50</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>25</v>
+      </c>
+      <c r="J7" s="8">
+        <v>75</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>96</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>67</v>
+      </c>
+      <c r="J8" s="8">
+        <v>163</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>59</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>37</v>
+      </c>
+      <c r="J9" s="8">
+        <v>96</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>39</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>73</v>
+      </c>
+      <c r="J10" s="8">
+        <v>112</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>10</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>86</v>
+      </c>
+      <c r="J11" s="8">
+        <v>96</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>91</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8">
+        <v>92</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>8</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>59</v>
+      </c>
+      <c r="J13" s="8">
+        <v>67</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>78</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>38</v>
+      </c>
+      <c r="J14" s="10">
+        <v>116</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>84</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>58</v>
+      </c>
+      <c r="J20" s="14">
+        <v>26</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>18</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>27</v>
+      </c>
+      <c r="J21" s="18">
+        <v>-9</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>15</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>53</v>
+      </c>
+      <c r="J22" s="18">
+        <v>-38</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>9</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>18</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>73</v>
+      </c>
+      <c r="J23" s="18">
+        <v>-55</v>
+      </c>
+      <c r="K23" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>44</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>7</v>
+      </c>
+      <c r="J24" s="18">
+        <v>37</v>
+      </c>
+      <c r="K24" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>65</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>34</v>
+      </c>
+      <c r="J25" s="18">
+        <v>31</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>9</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>8</v>
+      </c>
+      <c r="J26" s="18">
+        <v>1</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>61</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>31</v>
+      </c>
+      <c r="J27" s="18">
+        <v>30</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>98</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>88</v>
+      </c>
+      <c r="J28" s="18">
+        <v>10</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>61</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>85</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-24</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>97</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>27</v>
+      </c>
+      <c r="J30" s="22">
+        <v>70</v>
+      </c>
+      <c r="K30" s="19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>23</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>20</v>
+      </c>
+      <c r="J36" s="14">
+        <v>460</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>23</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>12</v>
+      </c>
+      <c r="J37" s="18">
+        <v>276</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>19</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>7</v>
+      </c>
+      <c r="J38" s="18">
+        <v>133</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>16</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>15</v>
+      </c>
+      <c r="J39" s="18">
+        <v>240</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>25</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>17</v>
+      </c>
+      <c r="J40" s="18">
+        <v>425</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>12</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>21</v>
+      </c>
+      <c r="J41" s="18">
+        <v>252</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>10</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>14</v>
+      </c>
+      <c r="J42" s="18">
+        <v>140</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>18</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>2</v>
+      </c>
+      <c r="J43" s="18">
+        <v>36</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>1</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>24</v>
+      </c>
+      <c r="J44" s="18">
+        <v>24</v>
+      </c>
+      <c r="K44" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>10</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>25</v>
+      </c>
+      <c r="J45" s="18">
+        <v>250</v>
+      </c>
+      <c r="K45" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>2</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>16</v>
+      </c>
+      <c r="J46" s="22">
+        <v>32</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>16</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>8</v>
+      </c>
+      <c r="J52" s="23">
+        <v>2</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>28</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>13</v>
+      </c>
+      <c r="J53" s="18">
+        <v>2.15</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>12</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>18</v>
+      </c>
+      <c r="J54" s="18">
+        <v>0.67</v>
+      </c>
+      <c r="K54" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>12</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>6</v>
+      </c>
+      <c r="J55" s="18">
+        <v>2</v>
+      </c>
+      <c r="K55" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>25</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>29</v>
+      </c>
+      <c r="J56" s="18">
+        <v>0.86</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>8</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>24</v>
+      </c>
+      <c r="J57" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K57" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>21</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>28</v>
+      </c>
+      <c r="J58" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="K58" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>23</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>21</v>
+      </c>
+      <c r="J59" s="18">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>29</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>28</v>
+      </c>
+      <c r="J60" s="18">
+        <v>1.04</v>
+      </c>
+      <c r="K60" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>5</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>9</v>
+      </c>
+      <c r="J61" s="18">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K61" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>5</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>27</v>
+      </c>
+      <c r="J62" s="22">
+        <v>0.19</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{6C3F38F3-DD76-4E29-853B-2A4D30137A0A}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{269E48F8-169F-4145-8618-570F8EF11BFD}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{DFBC4B5C-0207-4B01-BAA6-D68254A43DBE}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{5EE3699A-FA5F-41FD-B79F-F852245A17EE}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
@@ -6693,14 +8148,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -6709,15 +8164,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -6745,15 +8200,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -6783,15 +8238,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -6816,15 +8271,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -6849,15 +8304,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -6882,15 +8337,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -6915,15 +8370,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -6948,15 +8403,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -6981,15 +8436,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -7014,15 +8469,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -7047,15 +8502,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -7091,14 +8546,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -7366,14 +8821,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="61" t="s">
+      <c r="F34" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -7588,14 +9043,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-6
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCD07C1-739A-485B-9256-3F7995FC9D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83266B-AF8F-4AE0-A20D-D57F9D21961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Hari Ke-3" sheetId="4" r:id="rId3"/>
     <sheet name="Hari Ke-4" sheetId="5" r:id="rId4"/>
     <sheet name="Hari Ke-5" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="Hari Ke-6" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
@@ -26,7 +27,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Hari Ke-3'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Hari Ke-4'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Hari Ke-5'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Hari Ke-6'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -412,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -574,6 +576,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -943,14 +957,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -959,15 +973,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -995,11 +1009,11 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -1033,15 +1047,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1071,15 +1085,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1109,15 +1123,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1147,15 +1161,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1185,15 +1199,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1223,15 +1237,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1261,15 +1275,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1299,15 +1313,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1337,15 +1351,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1391,14 +1405,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1716,14 +1730,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="65" t="s">
+      <c r="F34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -1988,14 +2002,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="66" t="s">
+      <c r="F50" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2384,14 +2398,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2400,15 +2414,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>1</v>
@@ -2436,15 +2450,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2474,15 +2488,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2512,15 +2526,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2550,15 +2564,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2588,15 +2602,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2626,15 +2640,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2664,15 +2678,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2702,15 +2716,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2740,15 +2754,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2778,15 +2792,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2832,14 +2846,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -3157,14 +3171,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="65" t="s">
+      <c r="F34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3429,14 +3443,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="66" t="s">
+      <c r="F50" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -3825,14 +3839,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3841,15 +3855,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>1</v>
@@ -3877,7 +3891,7 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
@@ -3885,7 +3899,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -3915,15 +3929,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -3953,15 +3967,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -3991,15 +4005,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -4029,15 +4043,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>21</v>
-      </c>
-      <c r="C8" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>12</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -4067,15 +4081,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -4105,7 +4119,7 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -4113,7 +4127,7 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -4143,15 +4157,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -4181,15 +4195,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -4219,15 +4233,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -4273,14 +4287,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -4598,14 +4612,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="65" t="s">
+      <c r="F34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -4870,14 +4884,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="66" t="s">
+      <c r="F50" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -5266,14 +5280,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5282,15 +5296,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F3" s="54" t="s">
         <v>1</v>
@@ -5318,15 +5332,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -5356,15 +5370,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -5394,15 +5408,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>28</v>
-      </c>
-      <c r="C6" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>27</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -5432,15 +5446,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -5470,7 +5484,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -5478,7 +5492,7 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -5508,15 +5522,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -5546,15 +5560,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -5584,15 +5598,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -5622,15 +5636,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -5660,15 +5674,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -5714,14 +5728,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -6039,14 +6053,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="65" t="s">
+      <c r="F34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -6311,14 +6325,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="66" t="s">
+      <c r="F50" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -6680,7 +6694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA416E0B-43CD-4AE8-B502-D513E78B933D}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -6707,14 +6721,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -6723,15 +6737,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>1</v>
@@ -6759,15 +6773,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -6797,15 +6811,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -6835,15 +6849,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -6873,15 +6887,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -6911,15 +6925,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -6949,15 +6963,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -6987,15 +7001,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -7025,15 +7039,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -7063,15 +7077,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -7101,15 +7115,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -7155,14 +7169,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -7480,14 +7494,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="65" t="s">
+      <c r="F34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -7752,14 +7766,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="66" t="s">
+      <c r="F50" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -8118,6 +8132,1447 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17373CD-2DAD-4582-9E2F-F47F97193A60}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>25</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>25</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>22</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>10</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>19</v>
+      </c>
+      <c r="J4" s="6">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>99</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>16</v>
+      </c>
+      <c r="J5" s="8">
+        <v>115</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>29</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>73</v>
+      </c>
+      <c r="J6" s="8">
+        <v>102</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>11</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>65</v>
+      </c>
+      <c r="J7" s="8">
+        <v>76</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>48</v>
+      </c>
+      <c r="J8" s="8">
+        <v>75</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>8</v>
+      </c>
+      <c r="J9" s="8">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>36</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>95</v>
+      </c>
+      <c r="J10" s="8">
+        <v>131</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>76</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>34</v>
+      </c>
+      <c r="J11" s="8">
+        <v>110</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>12</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>53</v>
+      </c>
+      <c r="J12" s="8">
+        <v>65</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>39</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>24</v>
+      </c>
+      <c r="J13" s="8">
+        <v>63</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>71</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>72</v>
+      </c>
+      <c r="J14" s="10">
+        <v>143</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>65</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>55</v>
+      </c>
+      <c r="J20" s="14">
+        <v>10</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>48</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>66</v>
+      </c>
+      <c r="J21" s="18">
+        <v>-18</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>10</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>84</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>11</v>
+      </c>
+      <c r="J22" s="18">
+        <v>73</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>29</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>28</v>
+      </c>
+      <c r="J23" s="18">
+        <v>1</v>
+      </c>
+      <c r="K23" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>92</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>79</v>
+      </c>
+      <c r="J24" s="18">
+        <v>13</v>
+      </c>
+      <c r="K24" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>71</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>87</v>
+      </c>
+      <c r="J25" s="18">
+        <v>-16</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>34</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>48</v>
+      </c>
+      <c r="J26" s="18">
+        <v>-14</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>1</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>70</v>
+      </c>
+      <c r="J27" s="18">
+        <v>-69</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>74</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>94</v>
+      </c>
+      <c r="J28" s="18">
+        <v>-20</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>5</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>93</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-88</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>37</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>85</v>
+      </c>
+      <c r="J30" s="22">
+        <v>-48</v>
+      </c>
+      <c r="K30" s="19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>11</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>15</v>
+      </c>
+      <c r="J36" s="14">
+        <v>165</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>10</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>17</v>
+      </c>
+      <c r="J37" s="18">
+        <v>170</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>9</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>5</v>
+      </c>
+      <c r="J38" s="18">
+        <v>45</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>15</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>15</v>
+      </c>
+      <c r="J39" s="18">
+        <v>225</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>16</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>29</v>
+      </c>
+      <c r="J40" s="18">
+        <v>464</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>24</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>2</v>
+      </c>
+      <c r="J41" s="18">
+        <v>48</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>28</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>29</v>
+      </c>
+      <c r="J42" s="18">
+        <v>522</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>14</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>13</v>
+      </c>
+      <c r="J43" s="18">
+        <v>182</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>29</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>7</v>
+      </c>
+      <c r="J44" s="18">
+        <v>203</v>
+      </c>
+      <c r="K44" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>1</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>12</v>
+      </c>
+      <c r="J45" s="18">
+        <v>12</v>
+      </c>
+      <c r="K45" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>22</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>19</v>
+      </c>
+      <c r="J46" s="22">
+        <v>418</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>26</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>22</v>
+      </c>
+      <c r="J52" s="23">
+        <v>1.18</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>7</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>22</v>
+      </c>
+      <c r="J53" s="18">
+        <v>0.32</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>5</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>27</v>
+      </c>
+      <c r="J54" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="K54" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>18</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>23</v>
+      </c>
+      <c r="J55" s="18">
+        <v>0.78</v>
+      </c>
+      <c r="K55" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>13</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>16</v>
+      </c>
+      <c r="J56" s="18">
+        <v>0.81</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>9</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>6</v>
+      </c>
+      <c r="J57" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="K57" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>29</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>15</v>
+      </c>
+      <c r="J58" s="18">
+        <v>1.93</v>
+      </c>
+      <c r="K58" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>2</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>15</v>
+      </c>
+      <c r="J59" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>15</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>11</v>
+      </c>
+      <c r="J60" s="18">
+        <v>1.36</v>
+      </c>
+      <c r="K60" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>6</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>24</v>
+      </c>
+      <c r="J61" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="K61" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>1</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>4</v>
+      </c>
+      <c r="J62" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{55EBA245-B4E6-4056-900F-D4006201C89C}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{DD7097DF-6115-4077-8212-C7A3447FBBC8}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{342FBCC8-3162-4972-BBE2-F5A2755DF054}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{8DE4F249-044F-4798-BB8B-70D78234324D}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
@@ -8148,14 +9603,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -8164,15 +9619,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -8200,15 +9655,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -8238,15 +9693,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -8271,15 +9726,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -8304,15 +9759,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -8337,15 +9792,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -8370,15 +9825,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -8403,15 +9858,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -8436,15 +9891,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -8469,15 +9924,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -8502,15 +9957,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -8546,14 +10001,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -8821,14 +10276,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="65" t="s">
+      <c r="F34" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -9043,14 +10498,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="66" t="s">
+      <c r="F50" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="66"/>
+      <c r="G50" s="70"/>
+      <c r="H50" s="70"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="70"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-7
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83266B-AF8F-4AE0-A20D-D57F9D21961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65B3928-AC64-4DCD-9B9B-A62F93C370FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Hari Ke-4" sheetId="5" r:id="rId4"/>
     <sheet name="Hari Ke-5" sheetId="6" r:id="rId5"/>
     <sheet name="Hari Ke-6" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Hari Ke-7" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
@@ -28,7 +29,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Hari Ke-4'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Hari Ke-5'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Hari Ke-6'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Hari Ke-7'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -414,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -576,6 +578,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,14 +971,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -973,15 +987,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -1009,15 +1023,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -1047,15 +1061,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>21</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1085,15 +1099,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1123,15 +1137,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1161,15 +1175,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1199,15 +1213,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1237,15 +1251,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -1275,15 +1289,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>26</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>22</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1313,15 +1327,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1351,15 +1365,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1405,14 +1419,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1730,14 +1744,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -2002,14 +2016,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2398,14 +2412,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2414,15 +2428,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>1</v>
@@ -2450,15 +2464,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2488,15 +2502,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2526,15 +2540,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2564,15 +2578,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2602,15 +2616,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2640,15 +2654,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2678,15 +2692,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>28</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>25</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2716,15 +2730,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2754,15 +2768,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2792,15 +2806,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2846,14 +2860,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -3171,14 +3185,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3443,14 +3457,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -3839,14 +3853,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3855,15 +3869,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>1</v>
@@ -3891,15 +3905,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -3929,15 +3943,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -3967,15 +3981,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -4005,15 +4019,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -4043,15 +4057,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -4081,15 +4095,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -4119,15 +4133,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -4157,15 +4171,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -4195,15 +4209,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -4233,15 +4247,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -4287,14 +4301,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -4612,14 +4626,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -4884,14 +4898,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -5280,14 +5294,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5296,15 +5310,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F3" s="54" t="s">
         <v>1</v>
@@ -5332,15 +5346,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -5370,15 +5384,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -5408,15 +5422,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -5446,15 +5460,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -5484,15 +5498,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -5522,15 +5536,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -5560,15 +5574,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -5598,15 +5612,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
         <v>12</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>18</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -5636,15 +5650,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -5674,15 +5688,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -5728,14 +5742,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -6053,14 +6067,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -6325,14 +6339,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -6721,14 +6735,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -6737,15 +6751,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>1</v>
@@ -6773,15 +6787,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -6811,15 +6825,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -6849,15 +6863,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -6887,15 +6901,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -6925,15 +6939,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -6963,15 +6977,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -7001,15 +7015,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -7039,15 +7053,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -7077,15 +7091,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -7115,11 +7129,11 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -7169,14 +7183,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -7494,14 +7508,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -7766,14 +7780,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -8135,7 +8149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17373CD-2DAD-4582-9E2F-F47F97193A60}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -8162,14 +8176,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -8178,15 +8192,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F3" s="63" t="s">
         <v>1</v>
@@ -8214,15 +8228,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -8252,15 +8266,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -8290,15 +8304,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -8328,15 +8342,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -8366,15 +8380,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -8408,11 +8422,11 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -8442,15 +8456,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -8480,7 +8494,7 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -8488,7 +8502,7 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -8518,15 +8532,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -8556,15 +8570,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -8610,14 +8624,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -8935,14 +8949,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -9207,14 +9221,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -9573,6 +9587,1447 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA48056-55BB-48CF-939B-D50A96C598FA}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>98</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>7</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>77</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>27</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>71</v>
+      </c>
+      <c r="J4" s="6">
+        <v>85</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>17</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>34</v>
+      </c>
+      <c r="J5" s="8">
+        <v>51</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>93</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>32</v>
+      </c>
+      <c r="J6" s="8">
+        <v>125</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>64</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>60</v>
+      </c>
+      <c r="J7" s="8">
+        <v>124</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>49</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>84</v>
+      </c>
+      <c r="J8" s="8">
+        <v>133</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>71</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>59</v>
+      </c>
+      <c r="J9" s="8">
+        <v>130</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>81</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>28</v>
+      </c>
+      <c r="J10" s="8">
+        <v>109</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>99</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>76</v>
+      </c>
+      <c r="J11" s="8">
+        <v>175</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>97</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>67</v>
+      </c>
+      <c r="J12" s="8">
+        <v>164</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>33</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>55</v>
+      </c>
+      <c r="J13" s="8">
+        <v>88</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>60</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>47</v>
+      </c>
+      <c r="J14" s="10">
+        <v>107</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>2</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>34</v>
+      </c>
+      <c r="J20" s="14">
+        <v>-32</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>93</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>69</v>
+      </c>
+      <c r="J21" s="18">
+        <v>24</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>91</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>20</v>
+      </c>
+      <c r="J22" s="18">
+        <v>71</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>10</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>38</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>81</v>
+      </c>
+      <c r="J23" s="18">
+        <v>-43</v>
+      </c>
+      <c r="K23" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>21</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>76</v>
+      </c>
+      <c r="J24" s="18">
+        <v>-55</v>
+      </c>
+      <c r="K24" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>58</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>94</v>
+      </c>
+      <c r="J25" s="18">
+        <v>-36</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>83</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>48</v>
+      </c>
+      <c r="J26" s="18">
+        <v>35</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>50</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>40</v>
+      </c>
+      <c r="J27" s="18">
+        <v>10</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>98</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>82</v>
+      </c>
+      <c r="J28" s="18">
+        <v>16</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>57</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>84</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-27</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>41</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>43</v>
+      </c>
+      <c r="J30" s="22">
+        <v>-2</v>
+      </c>
+      <c r="K30" s="19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+    </row>
+    <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>14</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>22</v>
+      </c>
+      <c r="J36" s="14">
+        <v>308</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>20</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>23</v>
+      </c>
+      <c r="J37" s="18">
+        <v>460</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>7</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>9</v>
+      </c>
+      <c r="J38" s="18">
+        <v>63</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>9</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>21</v>
+      </c>
+      <c r="J39" s="18">
+        <v>189</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>25</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>29</v>
+      </c>
+      <c r="J40" s="18">
+        <v>725</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>22</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>11</v>
+      </c>
+      <c r="J41" s="18">
+        <v>242</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>7</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>26</v>
+      </c>
+      <c r="J42" s="18">
+        <v>182</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>13</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>8</v>
+      </c>
+      <c r="J43" s="18">
+        <v>104</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>16</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>18</v>
+      </c>
+      <c r="J44" s="18">
+        <v>288</v>
+      </c>
+      <c r="K44" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>4</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>29</v>
+      </c>
+      <c r="J45" s="18">
+        <v>116</v>
+      </c>
+      <c r="K45" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>2</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>20</v>
+      </c>
+      <c r="J46" s="22">
+        <v>40</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>8</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>13</v>
+      </c>
+      <c r="J52" s="23">
+        <v>0.62</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>19</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>16</v>
+      </c>
+      <c r="J53" s="18">
+        <v>1.19</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>14</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>12</v>
+      </c>
+      <c r="J54" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="K54" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>13</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>13</v>
+      </c>
+      <c r="J55" s="18">
+        <v>1</v>
+      </c>
+      <c r="K55" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>27</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>14</v>
+      </c>
+      <c r="J56" s="18">
+        <v>1.93</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>11</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>30</v>
+      </c>
+      <c r="J57" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="K57" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>18</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>15</v>
+      </c>
+      <c r="J58" s="18">
+        <v>1.2</v>
+      </c>
+      <c r="K58" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>2</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>13</v>
+      </c>
+      <c r="J59" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>18</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>23</v>
+      </c>
+      <c r="J60" s="18">
+        <v>0.78</v>
+      </c>
+      <c r="K60" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>16</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>15</v>
+      </c>
+      <c r="J61" s="18">
+        <v>1.06</v>
+      </c>
+      <c r="K61" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>25</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>17</v>
+      </c>
+      <c r="J62" s="22">
+        <v>1.47</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{AD549D21-3D1F-4FF1-B596-BEE09E345E56}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{59A486DE-FA70-4F0C-86F0-6A0041EB79F0}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{FED0F7F7-4162-4211-AB22-5360F95B48C0}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{B237FC5A-64E5-40DC-8240-DDE648B80CEC}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
@@ -9603,14 +11058,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -9619,15 +11074,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -9655,15 +11110,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -9693,15 +11148,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -9726,7 +11181,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -9734,7 +11189,7 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -9759,15 +11214,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -9792,15 +11247,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -9825,15 +11280,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -9858,15 +11313,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -9891,15 +11346,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -9924,15 +11379,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -9957,15 +11412,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -10001,14 +11456,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="68" t="s">
+      <c r="F18" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -10276,14 +11731,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="69" t="s">
+      <c r="F34" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -10498,14 +11953,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="70" t="s">
+      <c r="F50" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>

<commit_message>
Update Pengerjaan latihan minggu ke-1 hari ke-8
</commit_message>
<xml_diff>
--- a/Latihan Minggu Ke-1.xlsx
+++ b/Latihan Minggu Ke-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Pembelajaran-dan-latihan-hitungan-dengan-mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65B3928-AC64-4DCD-9B9B-A62F93C370FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BADC4E4-7116-4B7B-A276-9814DD07D171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{CE347DA0-4D35-403C-9B02-A84D6CBD4A6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hari Ke-1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Hari Ke-5" sheetId="6" r:id="rId5"/>
     <sheet name="Hari Ke-6" sheetId="7" r:id="rId6"/>
     <sheet name="Hari Ke-7" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId8"/>
+    <sheet name="Hari Ke-8" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hari Ke-1'!$F$19:$K$19</definedName>
@@ -30,7 +31,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Hari Ke-5'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Hari Ke-6'!$F$19:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Hari Ke-7'!$F$19:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sheet1!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Hari Ke-8'!$F$19:$K$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Sheet1!$F$19:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="24">
   <si>
     <t>Angka-angka acak untuk penjumlahan dan pengurangan</t>
   </si>
@@ -416,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -578,6 +580,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -971,14 +985,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -987,15 +1001,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -1023,15 +1037,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -1061,15 +1075,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -1099,15 +1113,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -1137,15 +1151,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -1175,15 +1189,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -1213,15 +1227,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -1251,11 +1265,11 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -1289,15 +1303,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -1327,15 +1341,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -1365,7 +1379,7 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -1373,7 +1387,7 @@
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -1419,14 +1433,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -1744,14 +1758,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -2016,14 +2030,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -2412,14 +2426,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -2428,15 +2442,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F3" s="46" t="s">
         <v>1</v>
@@ -2464,15 +2478,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -2502,15 +2516,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -2540,15 +2554,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -2578,7 +2592,7 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -2586,7 +2600,7 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -2616,15 +2630,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -2654,15 +2668,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -2692,15 +2706,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -2730,15 +2744,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -2768,15 +2782,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -2806,15 +2820,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -2860,14 +2874,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -3185,14 +3199,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -3457,14 +3471,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -3853,14 +3867,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3869,15 +3883,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>1</v>
@@ -3905,7 +3919,7 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
@@ -3943,7 +3957,7 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -3951,7 +3965,7 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -3981,15 +3995,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -4019,15 +4033,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -4057,15 +4071,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -4095,15 +4109,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -4133,15 +4147,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -4171,15 +4185,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -4209,15 +4223,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -4247,15 +4261,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -4301,14 +4315,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -4626,14 +4640,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -4898,14 +4912,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -5294,14 +5308,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -5310,15 +5324,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F3" s="54" t="s">
         <v>1</v>
@@ -5346,15 +5360,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -5384,15 +5398,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -5422,15 +5436,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -5460,15 +5474,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -5498,15 +5512,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -5536,15 +5550,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -5574,15 +5588,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -5612,15 +5626,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -5650,15 +5664,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -5688,15 +5702,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -5742,14 +5756,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -6067,14 +6081,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -6339,14 +6353,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -6735,14 +6749,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -6751,15 +6765,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>1</v>
@@ -6787,15 +6801,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -6825,15 +6839,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -6863,15 +6877,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -6901,15 +6915,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -6939,15 +6953,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -6977,15 +6991,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -7015,15 +7029,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -7053,15 +7067,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -7091,15 +7105,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -7129,15 +7143,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -7183,14 +7197,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -7508,14 +7522,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -7780,14 +7794,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -8176,14 +8190,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -8192,15 +8206,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F3" s="63" t="s">
         <v>1</v>
@@ -8228,15 +8242,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -8266,15 +8280,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -8304,15 +8318,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -8342,15 +8356,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -8380,15 +8394,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -8418,15 +8432,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -8456,15 +8470,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -8494,15 +8508,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -8532,15 +8546,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -8570,15 +8584,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -8624,14 +8638,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -8949,14 +8963,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -9221,14 +9235,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -9590,7 +9604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA48056-55BB-48CF-939B-D50A96C598FA}">
   <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
@@ -9617,14 +9631,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -9633,15 +9647,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F3" s="67" t="s">
         <v>1</v>
@@ -9669,15 +9683,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -9707,15 +9721,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -9745,7 +9759,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -9753,7 +9767,7 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -9783,15 +9797,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -9821,15 +9835,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -9859,15 +9873,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -9897,15 +9911,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -9935,15 +9949,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -9973,15 +9987,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -10011,15 +10025,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -10065,14 +10079,14 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -10390,14 +10404,14 @@
       </c>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -10662,14 +10676,14 @@
       </c>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">
@@ -11028,6 +11042,1451 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129B7757-5591-4426-B8BF-BCC9C3F71B80}">
+  <dimension ref="A2:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="33.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>55</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>30</v>
+      </c>
+      <c r="D3" s="2">
+        <f ca="1">RANDBETWEEN(1,25)</f>
+        <v>24</v>
+      </c>
+      <c r="F3" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A13" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
+        <v>79</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
+        <v>26</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>54</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5">
+        <v>59</v>
+      </c>
+      <c r="J4" s="6">
+        <v>113</v>
+      </c>
+      <c r="K4" s="5">
+        <f>IF((G4+I4)=J4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>94</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="7">
+        <v>77</v>
+      </c>
+      <c r="J5" s="8">
+        <v>171</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" ref="K5:K14" si="4">IF((G5+I5)=J5,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="7">
+        <v>68</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="7">
+        <v>24</v>
+      </c>
+      <c r="J6" s="8">
+        <v>92</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>20</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="7">
+        <v>14</v>
+      </c>
+      <c r="J7" s="8">
+        <v>34</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
+        <v>40</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>89</v>
+      </c>
+      <c r="J8" s="8">
+        <v>129</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>11</v>
+      </c>
+      <c r="J9" s="8">
+        <v>33</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G10" s="7">
+        <v>61</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="7">
+        <v>75</v>
+      </c>
+      <c r="J10" s="8">
+        <v>136</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>66</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="7">
+        <v>18</v>
+      </c>
+      <c r="J11" s="8">
+        <v>84</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="7">
+        <v>24</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7">
+        <v>93</v>
+      </c>
+      <c r="J12" s="8">
+        <v>117</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>78</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>94</v>
+      </c>
+      <c r="J13" s="8">
+        <v>172</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F14" s="9">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>94</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="9">
+        <v>39</v>
+      </c>
+      <c r="J14" s="10">
+        <v>133</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+    </row>
+    <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="37">
+        <f>COUNTIF($K$4:$K$14,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D20" s="43">
+        <f>COUNTIF($K$4:$K$14,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <v>29</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>97</v>
+      </c>
+      <c r="J20" s="14">
+        <v>-68</v>
+      </c>
+      <c r="K20" s="11">
+        <f>IF((G20-I20)=J20,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="38">
+        <f>COUNTIF($K$20:$K$30,1)</f>
+        <v>11</v>
+      </c>
+      <c r="D21" s="44">
+        <f>COUNTIF($K$20:$K$30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" ref="F21:F30" si="5">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>72</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="17">
+        <v>64</v>
+      </c>
+      <c r="J21" s="18">
+        <v>8</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" ref="K21:K30" si="6">IF((G21-I21)=J21,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="38">
+        <f>COUNTIF($K$36:$K$46,1)</f>
+        <v>10</v>
+      </c>
+      <c r="D22" s="44">
+        <f>COUNTIF($K$36:$K$46,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G22" s="16">
+        <v>63</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="17">
+        <v>88</v>
+      </c>
+      <c r="J22" s="18">
+        <v>-25</v>
+      </c>
+      <c r="K22" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="39">
+        <f>COUNTIF($K$52:$K$62,1)</f>
+        <v>10</v>
+      </c>
+      <c r="D23" s="45">
+        <f>COUNTIF($K$52:$K$62,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="16">
+        <v>20</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="17">
+        <v>81</v>
+      </c>
+      <c r="J23" s="18">
+        <v>-61</v>
+      </c>
+      <c r="K23" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="16">
+        <v>36</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="17">
+        <v>86</v>
+      </c>
+      <c r="J24" s="18">
+        <v>-50</v>
+      </c>
+      <c r="K24" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F25" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="16">
+        <v>43</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="17">
+        <v>80</v>
+      </c>
+      <c r="J25" s="18">
+        <v>-37</v>
+      </c>
+      <c r="K25" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F26" s="15">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="G26" s="16">
+        <v>35</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="17">
+        <v>18</v>
+      </c>
+      <c r="J26" s="18">
+        <v>17</v>
+      </c>
+      <c r="K26" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F27" s="15">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="16">
+        <v>74</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="17">
+        <v>76</v>
+      </c>
+      <c r="J27" s="18">
+        <v>-2</v>
+      </c>
+      <c r="K27" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F28" s="15">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="G28" s="16">
+        <v>77</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="17">
+        <v>3</v>
+      </c>
+      <c r="J28" s="18">
+        <v>74</v>
+      </c>
+      <c r="K28" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F29" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="16">
+        <v>41</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" s="17">
+        <v>42</v>
+      </c>
+      <c r="J29" s="18">
+        <v>-1</v>
+      </c>
+      <c r="K29" s="15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F30" s="19">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="G30" s="20">
+        <v>19</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="21">
+        <v>89</v>
+      </c>
+      <c r="J30" s="22">
+        <v>-70</v>
+      </c>
+      <c r="K30" s="19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+    </row>
+    <row r="35" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F36" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>13</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="13">
+        <v>24</v>
+      </c>
+      <c r="J36" s="14">
+        <v>312</v>
+      </c>
+      <c r="K36" s="11">
+        <f>IF((G36*I36)=J36,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F37" s="15">
+        <f t="shared" ref="F37:F46" si="7">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G37" s="16">
+        <v>16</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="17">
+        <v>9</v>
+      </c>
+      <c r="J37" s="18">
+        <v>144</v>
+      </c>
+      <c r="K37" s="15">
+        <f t="shared" ref="K37:K46" si="8">IF((G37*I37)=J37,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F38" s="15">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G38" s="16">
+        <v>4</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="17">
+        <v>2</v>
+      </c>
+      <c r="J38" s="18">
+        <v>8</v>
+      </c>
+      <c r="K38" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F39" s="15">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G39" s="16">
+        <v>6</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="17">
+        <v>25</v>
+      </c>
+      <c r="J39" s="18">
+        <v>150</v>
+      </c>
+      <c r="K39" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <f>24*17</f>
+        <v>408</v>
+      </c>
+      <c r="F40" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G40" s="16">
+        <v>24</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="17">
+        <v>17</v>
+      </c>
+      <c r="J40" s="18">
+        <v>388</v>
+      </c>
+      <c r="K40" s="15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F41" s="15">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G41" s="16">
+        <v>5</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="17">
+        <v>16</v>
+      </c>
+      <c r="J41" s="18">
+        <v>80</v>
+      </c>
+      <c r="K41" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F42" s="15">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="16">
+        <v>1</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="17">
+        <v>10</v>
+      </c>
+      <c r="J42" s="18">
+        <v>10</v>
+      </c>
+      <c r="K42" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F43" s="15">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="16">
+        <v>12</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="17">
+        <v>29</v>
+      </c>
+      <c r="J43" s="18">
+        <v>348</v>
+      </c>
+      <c r="K43" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F44" s="15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="G44" s="16">
+        <v>22</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="17">
+        <v>27</v>
+      </c>
+      <c r="J44" s="18">
+        <v>594</v>
+      </c>
+      <c r="K44" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F45" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="16">
+        <v>4</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="17">
+        <v>11</v>
+      </c>
+      <c r="J45" s="18">
+        <v>44</v>
+      </c>
+      <c r="K45" s="15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F46" s="19">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="G46" s="20">
+        <v>18</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="21">
+        <v>9</v>
+      </c>
+      <c r="J46" s="22">
+        <v>162</v>
+      </c>
+      <c r="K46" s="19">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
+    </row>
+    <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="J51" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F52" s="11">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="G52" s="12">
+        <v>17</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13">
+        <v>3</v>
+      </c>
+      <c r="J52" s="23">
+        <v>5.67</v>
+      </c>
+      <c r="K52" s="11">
+        <f>IF(ROUND((G52/I52),2)=J52,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F53" s="15">
+        <f t="shared" ref="F53:F62" si="9">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="G53" s="16">
+        <v>24</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="17">
+        <v>11</v>
+      </c>
+      <c r="J53" s="18">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K53" s="15">
+        <f t="shared" ref="K53:K62" si="10">IF(ROUND((G53/I53),2)=J53,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F54" s="15">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="G54" s="16">
+        <v>20</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="17">
+        <v>17</v>
+      </c>
+      <c r="J54" s="18">
+        <v>1.18</v>
+      </c>
+      <c r="K54" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F55" s="15">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="16">
+        <v>25</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="17">
+        <v>14</v>
+      </c>
+      <c r="J55" s="18">
+        <v>1.79</v>
+      </c>
+      <c r="K55" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F56" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="G56" s="16">
+        <v>25</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="17">
+        <v>25</v>
+      </c>
+      <c r="J56" s="18">
+        <v>1</v>
+      </c>
+      <c r="K56" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F57" s="15">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G57" s="16">
+        <v>22</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="17">
+        <v>27</v>
+      </c>
+      <c r="J57" s="18">
+        <v>0.81</v>
+      </c>
+      <c r="K57" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F58" s="15">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G58" s="16">
+        <v>28</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="17">
+        <v>19</v>
+      </c>
+      <c r="J58" s="18">
+        <v>1.47</v>
+      </c>
+      <c r="K58" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F59" s="15">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="G59" s="16">
+        <v>28</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="17">
+        <v>15</v>
+      </c>
+      <c r="J59" s="18">
+        <v>1.87</v>
+      </c>
+      <c r="K59" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F60" s="15">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="G60" s="16">
+        <v>15</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="17">
+        <v>17</v>
+      </c>
+      <c r="J60" s="18">
+        <v>0.87</v>
+      </c>
+      <c r="K60" s="15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F61" s="15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="16">
+        <v>20</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="17">
+        <v>14</v>
+      </c>
+      <c r="J61" s="18">
+        <v>1.43</v>
+      </c>
+      <c r="K61" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="6:11" ht="18" x14ac:dyDescent="0.3">
+      <c r="F62" s="19">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="G62" s="20">
+        <v>15</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="21">
+        <v>18</v>
+      </c>
+      <c r="J62" s="22">
+        <v>0.83</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="F50:K50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{F3FA9424-29C6-457E-9AEC-ABAA3FA9E683}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K4:K14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{63E0A3D1-D13B-4C79-8E9A-8132856C05EF}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K20:K30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{D9D96050-2A07-4D7D-9892-839C17424111}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K36:K46</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{84AC8CCE-4B1C-4904-B675-DFB107A6D803}">
+            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K52:K62</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F971E95-2EF7-4A60-9BD8-C0B8F85947BF}">
   <dimension ref="A2:K62"/>
   <sheetViews>
@@ -11058,14 +12517,14 @@
       <c r="D2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -11074,15 +12533,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">RANDBETWEEN(1,25)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>1</v>
@@ -11110,15 +12569,15 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B13" ca="1" si="1">RANDBETWEEN(1,100)</f>
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ref="C4:D13" ca="1" si="2">RANDBETWEEN(1,30)</f>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5">
         <f>ROW(A1)</f>
@@ -11148,15 +12607,15 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" ref="F5:F14" si="3">ROW(A2)</f>
@@ -11181,15 +12640,15 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="3"/>
@@ -11214,15 +12673,15 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="3"/>
@@ -11247,15 +12706,15 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="3"/>
@@ -11280,15 +12739,15 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="3"/>
@@ -11313,15 +12772,15 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="3"/>
@@ -11346,15 +12805,15 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="3"/>
@@ -11379,15 +12838,15 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="3"/>
@@ -11412,15 +12871,15 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="3"/>
@@ -11456,14 +12915,14 @@
       <c r="K14" s="9"/>
     </row>
     <row r="18" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="2:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
@@ -11731,14 +13190,14 @@
       <c r="K30" s="19"/>
     </row>
     <row r="34" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
     </row>
     <row r="35" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
@@ -11953,14 +13412,14 @@
       <c r="K46" s="19"/>
     </row>
     <row r="50" spans="6:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="74" t="s">
+      <c r="F50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
     </row>
     <row r="51" spans="6:11" ht="18" x14ac:dyDescent="0.3">
       <c r="F51" s="26" t="s">

</xml_diff>